<commit_message>
Adds new classes and uses inhariteance
</commit_message>
<xml_diff>
--- a/Remote_Key_Function_Map.xlsx
+++ b/Remote_Key_Function_Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1230935be65cd61/Documents/Arduino/Bluetooth_Obstacle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{A35FD146-F317-4AEA-ADFA-DB93BA8194EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F895257F-3681-4595-BEDD-72204A66F0B4}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="8_{A35FD146-F317-4AEA-ADFA-DB93BA8194EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AB6284F-D098-4989-8EB5-B8BCFC585497}"/>
   <bookViews>
-    <workbookView xWindow="13425" yWindow="1470" windowWidth="43200" windowHeight="17145" activeTab="1" xr2:uid="{C798FCE4-2EFF-492E-8AB3-EFB167353297}"/>
+    <workbookView xWindow="5910" yWindow="3075" windowWidth="21600" windowHeight="17145" xr2:uid="{C798FCE4-2EFF-492E-8AB3-EFB167353297}"/>
   </bookViews>
   <sheets>
     <sheet name="Key_Map" sheetId="1" r:id="rId1"/>
@@ -85,9 +85,6 @@
     <t>Enable Obstacle Mode</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>EEPROM</t>
+  </si>
+  <si>
+    <t>Reset Step Size</t>
   </si>
 </sst>
 </file>
@@ -498,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8D3BEE-0351-43FE-89B2-835F77E95BA2}">
   <dimension ref="B1:T12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:N1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,7 +532,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
@@ -549,7 +549,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
@@ -566,7 +566,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
@@ -583,7 +583,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
@@ -600,7 +600,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
@@ -617,7 +617,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
@@ -634,7 +634,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:20" ht="30" x14ac:dyDescent="0.25">
@@ -648,10 +648,10 @@
         <v>54</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:20" ht="45" x14ac:dyDescent="0.25">
@@ -665,10 +665,10 @@
         <v>56</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:20" ht="45" x14ac:dyDescent="0.25">
@@ -682,10 +682,10 @@
         <v>57</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
@@ -699,7 +699,7 @@
         <v>48</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -716,7 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2936882C-42D6-4FD1-ACDD-761A7DC76302}">
   <dimension ref="A1:B252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -728,10 +728,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
         <v>25</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adds CMD for Look Left, Right and Around
adds CMD for Look Left, Right and Around
</commit_message>
<xml_diff>
--- a/Remote_Key_Function_Map.xlsx
+++ b/Remote_Key_Function_Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1230935be65cd61/Documents/Arduino/Bluetooth_Obstacle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="8_{A35FD146-F317-4AEA-ADFA-DB93BA8194EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AB6284F-D098-4989-8EB5-B8BCFC585497}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="8_{A35FD146-F317-4AEA-ADFA-DB93BA8194EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F3812D2-6199-4468-80C3-B789FAF13537}"/>
   <bookViews>
-    <workbookView xWindow="5910" yWindow="3075" windowWidth="21600" windowHeight="17145" xr2:uid="{C798FCE4-2EFF-492E-8AB3-EFB167353297}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="43200" windowHeight="17145" xr2:uid="{C798FCE4-2EFF-492E-8AB3-EFB167353297}"/>
   </bookViews>
   <sheets>
     <sheet name="Key_Map" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t xml:space="preserve">Forward </t>
   </si>
@@ -116,6 +116,27 @@
   </si>
   <si>
     <t>Reset Step Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look Left </t>
+  </si>
+  <si>
+    <t>Look Right</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Testing Option does not map to app Button</t>
+  </si>
+  <si>
+    <t>Look Back</t>
   </si>
 </sst>
 </file>
@@ -151,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -161,6 +182,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -186,8 +210,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C6380B5-67BE-4B07-8C4F-34574DE906A2}" name="Table1" displayName="Table1" ref="B2:F12" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="B2:F12" xr:uid="{1C6380B5-67BE-4B07-8C4F-34574DE906A2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C6380B5-67BE-4B07-8C4F-34574DE906A2}" name="Table1" displayName="Table1" ref="B2:F15" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="B2:F15" xr:uid="{1C6380B5-67BE-4B07-8C4F-34574DE906A2}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{53B31554-FE7B-4E71-AE54-9D49B70E1AF7}" name="Direction" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{BEEFE3CB-F606-4F56-923D-CFA3F44C51B9}" name="App Setting" dataDxfId="1" dataCellStyle="Normal"/>
@@ -496,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8D3BEE-0351-43FE-89B2-835F77E95BA2}">
-  <dimension ref="B1:T12"/>
+  <dimension ref="B1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,6 +726,57 @@
         <v>26</v>
       </c>
       <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="5">
+        <v>76</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="5">
+        <v>82</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="5">
+        <v>65</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>